<commit_message>
1. Bug Fix: 修复导出原生类型数组时的错误。 Fixed a bug when exporting an array of native types.
</commit_message>
<xml_diff>
--- a/res/source/proto.xlsx
+++ b/res/source/proto.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="30">
   <si>
     <t>协议Id</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -139,6 +139,10 @@
   </si>
   <si>
     <t>c4:[]*C</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>d:[]uint8</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -543,7 +547,7 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I15:I16"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -635,7 +639,7 @@
         <v>6</v>
       </c>
       <c r="E5" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:9">

</xml_diff>